<commit_message>
some changed after dp4
</commit_message>
<xml_diff>
--- a/data_processing/앱 분류 리스트.xlsx
+++ b/data_processing/앱 분류 리스트.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runni\Documents\cs481\cs481-dp\cs481-knowStress\data_processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0E0BAE-3C0C-47D7-97F8-665D3E976308}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17E785D-71C3-459A-B2A9-6515BAB12143}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{0B8AA2B1-9CFA-446A-B5B3-4B25F538EE4F}"/>
   </bookViews>
@@ -1575,7 +1575,7 @@
   <dimension ref="A1:B393"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>